<commit_message>
Update new autocomplete to customer purchase order .
</commit_message>
<xml_diff>
--- a/form/Stock 01-06-18/01.xlsx
+++ b/form/Stock 01-06-18/01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppServ\www\erp_mvc\form\Stock 01-06-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE3F339D-EDFC-41C0-A2EC-457B9532B549}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3493D6A1-E776-4263-A225-790548A8E998}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{39ABE9FA-C038-4EB7-B752-F5BBE2A7131D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
   <si>
     <t>100834  </t>
   </si>
@@ -549,12 +549,6 @@
     <t>Z16ER1.5ISO AZ203  </t>
   </si>
   <si>
-    <t>Z16IR1.0ISO AZ203  </t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
     <t>qty</t>
   </si>
   <si>
@@ -562,6 +556,9 @@
   </si>
   <si>
     <t>price_total</t>
+  </si>
+  <si>
+    <t>product_code</t>
   </si>
 </sst>
 </file>
@@ -586,7 +583,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -596,12 +593,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -633,12 +624,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -961,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F4EE5F-5937-4C8C-8851-2E986A5DD688}">
-  <dimension ref="A1:G1390"/>
+  <dimension ref="A1:E1367"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="K180" sqref="K180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18" customHeight="1"/>
@@ -974,23 +959,21 @@
     <col min="3" max="3" width="11.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1">
@@ -3231,7 +3214,7 @@
         <v>3424</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="18" customHeight="1">
+    <row r="161" spans="1:5" ht="18" customHeight="1">
       <c r="A161" s="3" t="s">
         <v>157</v>
       </c>
@@ -3245,7 +3228,7 @@
         <v>2690.16</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="18" customHeight="1">
+    <row r="162" spans="1:5" ht="18" customHeight="1">
       <c r="A162" s="3" t="s">
         <v>158</v>
       </c>
@@ -3260,7 +3243,7 @@
       </c>
       <c r="E162" s="5"/>
     </row>
-    <row r="163" spans="1:7" ht="18" customHeight="1">
+    <row r="163" spans="1:5" ht="18" customHeight="1">
       <c r="A163" s="3" t="s">
         <v>159</v>
       </c>
@@ -3275,7 +3258,7 @@
       </c>
       <c r="E163" s="5"/>
     </row>
-    <row r="164" spans="1:7" ht="18" customHeight="1">
+    <row r="164" spans="1:5" ht="18" customHeight="1">
       <c r="A164" s="3" t="s">
         <v>160</v>
       </c>
@@ -3289,7 +3272,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="18" customHeight="1">
+    <row r="165" spans="1:5" ht="18" customHeight="1">
       <c r="A165" s="3" t="s">
         <v>161</v>
       </c>
@@ -3304,7 +3287,7 @@
       </c>
       <c r="E165" s="5"/>
     </row>
-    <row r="166" spans="1:7" ht="18" customHeight="1">
+    <row r="166" spans="1:5" ht="18" customHeight="1">
       <c r="A166" s="3" t="s">
         <v>162</v>
       </c>
@@ -3318,7 +3301,7 @@
         <v>43411.8</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="18" customHeight="1">
+    <row r="167" spans="1:5" ht="18" customHeight="1">
       <c r="A167" s="3" t="s">
         <v>163</v>
       </c>
@@ -3332,7 +3315,7 @@
         <v>65410.8</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="18" customHeight="1">
+    <row r="168" spans="1:5" ht="18" customHeight="1">
       <c r="A168" s="3" t="s">
         <v>164</v>
       </c>
@@ -3346,7 +3329,7 @@
         <v>44787.16</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="18" customHeight="1">
+    <row r="169" spans="1:5" ht="18" customHeight="1">
       <c r="A169" s="3" t="s">
         <v>165</v>
       </c>
@@ -3360,7 +3343,7 @@
         <v>518.53</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="18" customHeight="1">
+    <row r="170" spans="1:5" ht="18" customHeight="1">
       <c r="A170" s="3" t="s">
         <v>166</v>
       </c>
@@ -3374,7 +3357,7 @@
         <v>5185.3</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="18" customHeight="1">
+    <row r="171" spans="1:5" ht="18" customHeight="1">
       <c r="A171" s="3" t="s">
         <v>167</v>
       </c>
@@ -3388,7 +3371,7 @@
         <v>15066.67</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="18" customHeight="1">
+    <row r="172" spans="1:5" ht="18" customHeight="1">
       <c r="A172" s="3" t="s">
         <v>168</v>
       </c>
@@ -3403,7 +3386,7 @@
       </c>
       <c r="E172" s="5"/>
     </row>
-    <row r="173" spans="1:7" ht="18" customHeight="1">
+    <row r="173" spans="1:5" ht="18" customHeight="1">
       <c r="A173" s="3" t="s">
         <v>169</v>
       </c>
@@ -3417,7 +3400,7 @@
         <v>10400</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="18" customHeight="1">
+    <row r="174" spans="1:5" ht="18" customHeight="1">
       <c r="A174" s="3" t="s">
         <v>170</v>
       </c>
@@ -3431,7 +3414,7 @@
         <v>21667.119999999999</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="18" customHeight="1">
+    <row r="175" spans="1:5" ht="18" customHeight="1">
       <c r="A175" s="3" t="s">
         <v>171</v>
       </c>
@@ -3444,10 +3427,8 @@
       <c r="D175" s="4">
         <v>47086.7</v>
       </c>
-      <c r="F175" s="6"/>
-      <c r="G175" s="6"/>
-    </row>
-    <row r="176" spans="1:7" ht="18" customHeight="1">
+    </row>
+    <row r="176" spans="1:5" ht="18" customHeight="1">
       <c r="A176" s="3" t="s">
         <v>172</v>
       </c>
@@ -3460,10 +3441,8 @@
       <c r="D176" s="4">
         <v>1298</v>
       </c>
-      <c r="F176" s="6"/>
-      <c r="G176" s="6"/>
-    </row>
-    <row r="177" spans="1:7" ht="18" customHeight="1">
+    </row>
+    <row r="177" spans="1:4" ht="18" customHeight="1">
       <c r="A177" s="3" t="s">
         <v>173</v>
       </c>
@@ -3476,559 +3455,487 @@
       <c r="D177" s="4">
         <v>4267.3100000000004</v>
       </c>
-      <c r="F177" s="6"/>
-      <c r="G177" s="6"/>
-    </row>
-    <row r="178" spans="1:7" ht="18" customHeight="1">
-      <c r="A178" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B178" s="2">
-        <v>63</v>
-      </c>
-      <c r="C178" s="2">
-        <v>200</v>
-      </c>
-      <c r="D178" s="4">
-        <v>12600</v>
-      </c>
-      <c r="F178" s="6"/>
-      <c r="G178" s="6"/>
-    </row>
-    <row r="179" spans="1:7" ht="18" customHeight="1">
-      <c r="G179" s="7"/>
-    </row>
-    <row r="180" spans="1:7" ht="18" customHeight="1">
-      <c r="G180" s="7"/>
-    </row>
-    <row r="182" spans="1:7" ht="18" customHeight="1">
-      <c r="D182" s="4"/>
-      <c r="E182" s="5"/>
-    </row>
-    <row r="185" spans="1:7" ht="18" customHeight="1">
-      <c r="C185" s="4"/>
-      <c r="D185" s="4"/>
-    </row>
-    <row r="186" spans="1:7" ht="18" customHeight="1">
-      <c r="C186" s="4"/>
+    </row>
+    <row r="186" spans="1:4" ht="18" customHeight="1">
       <c r="D186" s="4"/>
     </row>
-    <row r="187" spans="1:7" ht="18" customHeight="1">
-      <c r="C187" s="4"/>
+    <row r="187" spans="1:4" ht="18" customHeight="1">
       <c r="D187" s="4"/>
     </row>
-    <row r="189" spans="1:7" ht="18" customHeight="1">
-      <c r="D189" s="4"/>
-    </row>
-    <row r="190" spans="1:7" ht="18" customHeight="1">
+    <row r="190" spans="1:4" ht="18" customHeight="1">
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
     </row>
-    <row r="191" spans="1:7" ht="18" customHeight="1">
-      <c r="C191" s="4"/>
-      <c r="D191" s="4"/>
-    </row>
-    <row r="194" spans="3:7" ht="18" customHeight="1">
+    <row r="194" spans="3:4" ht="18" customHeight="1">
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
     </row>
-    <row r="197" spans="3:7" ht="18" customHeight="1">
-      <c r="G197" s="7"/>
-    </row>
-    <row r="209" spans="3:4" ht="18" customHeight="1">
-      <c r="D209" s="4"/>
-    </row>
-    <row r="210" spans="3:4" ht="18" customHeight="1">
-      <c r="D210" s="4"/>
-    </row>
-    <row r="213" spans="3:4" ht="18" customHeight="1">
-      <c r="C213" s="4"/>
-      <c r="D213" s="4"/>
-    </row>
-    <row r="217" spans="3:4" ht="18" customHeight="1">
-      <c r="C217" s="4"/>
-      <c r="D217" s="4"/>
-    </row>
-    <row r="219" spans="3:4" ht="18" customHeight="1">
-      <c r="C219" s="4"/>
-      <c r="D219" s="4"/>
-    </row>
-    <row r="220" spans="3:4" ht="18" customHeight="1">
-      <c r="D220" s="4"/>
-    </row>
-    <row r="221" spans="3:4" ht="18" customHeight="1">
-      <c r="D221" s="4"/>
-    </row>
-    <row r="223" spans="3:4" ht="18" customHeight="1">
-      <c r="C223" s="4"/>
-      <c r="D223" s="4"/>
-    </row>
-    <row r="238" spans="3:4" ht="18" customHeight="1">
-      <c r="D238" s="4"/>
-    </row>
-    <row r="239" spans="3:4" ht="18" customHeight="1">
-      <c r="C239" s="4"/>
-      <c r="D239" s="4"/>
-    </row>
-    <row r="242" spans="3:7" ht="18" customHeight="1">
-      <c r="G242" s="7"/>
-    </row>
-    <row r="247" spans="3:7" ht="18" customHeight="1">
-      <c r="C247" s="4"/>
+    <row r="196" spans="3:4" ht="18" customHeight="1">
+      <c r="C196" s="4"/>
+      <c r="D196" s="4"/>
+    </row>
+    <row r="197" spans="3:4" ht="18" customHeight="1">
+      <c r="D197" s="4"/>
+    </row>
+    <row r="198" spans="3:4" ht="18" customHeight="1">
+      <c r="D198" s="4"/>
+    </row>
+    <row r="200" spans="3:4" ht="18" customHeight="1">
+      <c r="C200" s="4"/>
+      <c r="D200" s="4"/>
+    </row>
+    <row r="215" spans="3:4" ht="18" customHeight="1">
+      <c r="D215" s="4"/>
+    </row>
+    <row r="216" spans="3:4" ht="18" customHeight="1">
+      <c r="C216" s="4"/>
+      <c r="D216" s="4"/>
+    </row>
+    <row r="224" spans="3:4" ht="18" customHeight="1">
+      <c r="C224" s="4"/>
+      <c r="D224" s="4"/>
+    </row>
+    <row r="227" spans="3:4" ht="18" customHeight="1">
+      <c r="C227" s="4"/>
+      <c r="D227" s="4"/>
+    </row>
+    <row r="228" spans="3:4" ht="18" customHeight="1">
+      <c r="C228" s="4"/>
+      <c r="D228" s="4"/>
+    </row>
+    <row r="229" spans="3:4" ht="18" customHeight="1">
+      <c r="D229" s="4"/>
+    </row>
+    <row r="230" spans="3:4" ht="18" customHeight="1">
+      <c r="D230" s="4"/>
+    </row>
+    <row r="231" spans="3:4" ht="18" customHeight="1">
+      <c r="D231" s="4"/>
+    </row>
+    <row r="234" spans="3:4" ht="18" customHeight="1">
+      <c r="C234" s="4"/>
+      <c r="D234" s="4"/>
+    </row>
+    <row r="235" spans="3:4" ht="18" customHeight="1">
+      <c r="C235" s="4"/>
+      <c r="D235" s="4"/>
+    </row>
+    <row r="236" spans="3:4" ht="18" customHeight="1">
+      <c r="C236" s="4"/>
+      <c r="D236" s="4"/>
+    </row>
+    <row r="247" spans="4:4" ht="18" customHeight="1">
       <c r="D247" s="4"/>
     </row>
-    <row r="250" spans="3:7" ht="18" customHeight="1">
-      <c r="C250" s="4"/>
-      <c r="D250" s="4"/>
-    </row>
-    <row r="251" spans="3:7" ht="18" customHeight="1">
-      <c r="C251" s="4"/>
+    <row r="251" spans="4:4" ht="18" customHeight="1">
       <c r="D251" s="4"/>
     </row>
-    <row r="252" spans="3:7" ht="18" customHeight="1">
-      <c r="D252" s="4"/>
-    </row>
-    <row r="253" spans="3:7" ht="18" customHeight="1">
-      <c r="D253" s="4"/>
-    </row>
-    <row r="254" spans="3:7" ht="18" customHeight="1">
-      <c r="D254" s="4"/>
-    </row>
-    <row r="257" spans="3:4" ht="18" customHeight="1">
-      <c r="C257" s="4"/>
-      <c r="D257" s="4"/>
-    </row>
-    <row r="258" spans="3:4" ht="18" customHeight="1">
-      <c r="C258" s="4"/>
-      <c r="D258" s="4"/>
-    </row>
-    <row r="259" spans="3:4" ht="18" customHeight="1">
-      <c r="C259" s="4"/>
-      <c r="D259" s="4"/>
-    </row>
-    <row r="270" spans="3:4" ht="18" customHeight="1">
-      <c r="D270" s="4"/>
-    </row>
-    <row r="274" spans="4:7" ht="18" customHeight="1">
-      <c r="D274" s="4"/>
-    </row>
-    <row r="283" spans="4:7" ht="18" customHeight="1">
-      <c r="D283" s="4"/>
-    </row>
-    <row r="287" spans="4:7" ht="18" customHeight="1">
-      <c r="G287" s="7"/>
-    </row>
-    <row r="292" spans="3:4" ht="18" customHeight="1">
-      <c r="C292" s="4"/>
-      <c r="D292" s="4"/>
-    </row>
-    <row r="295" spans="3:4" ht="18" customHeight="1">
-      <c r="D295" s="4"/>
-    </row>
-    <row r="314" spans="3:4" ht="18" customHeight="1">
-      <c r="C314" s="4"/>
-      <c r="D314" s="4"/>
-    </row>
-    <row r="328" spans="4:7" ht="18" customHeight="1">
-      <c r="D328" s="4"/>
-    </row>
-    <row r="332" spans="4:7" ht="18" customHeight="1">
-      <c r="G332" s="7"/>
-    </row>
-    <row r="352" spans="3:4" ht="18" customHeight="1">
-      <c r="C352" s="4"/>
-      <c r="D352" s="4"/>
-    </row>
-    <row r="356" spans="3:4" ht="18" customHeight="1">
-      <c r="D356" s="4"/>
-    </row>
-    <row r="359" spans="3:4" ht="18" customHeight="1">
-      <c r="C359" s="4"/>
-      <c r="D359" s="4"/>
-    </row>
-    <row r="360" spans="3:4" ht="18" customHeight="1">
-      <c r="C360" s="4"/>
-      <c r="D360" s="4"/>
-    </row>
-    <row r="370" spans="3:7" ht="18" customHeight="1">
-      <c r="C370" s="4"/>
-      <c r="D370" s="4"/>
-    </row>
-    <row r="377" spans="3:7" ht="18" customHeight="1">
-      <c r="G377" s="7"/>
-    </row>
-    <row r="399" spans="4:4" ht="18" customHeight="1">
-      <c r="D399" s="4"/>
-    </row>
-    <row r="408" spans="4:4" ht="18" customHeight="1">
-      <c r="D408" s="4"/>
-    </row>
-    <row r="410" spans="4:4" ht="18" customHeight="1">
-      <c r="D410" s="4"/>
-    </row>
-    <row r="413" spans="4:4" ht="18" customHeight="1">
-      <c r="D413" s="4"/>
-    </row>
-    <row r="418" spans="3:7" ht="18" customHeight="1">
-      <c r="D418" s="4"/>
-    </row>
-    <row r="419" spans="3:7" ht="18" customHeight="1">
-      <c r="D419" s="4"/>
-    </row>
-    <row r="422" spans="3:7" ht="18" customHeight="1">
-      <c r="G422" s="7"/>
-    </row>
-    <row r="428" spans="3:7" ht="18" customHeight="1">
-      <c r="C428" s="4"/>
-      <c r="D428" s="4"/>
-    </row>
-    <row r="437" spans="4:4" ht="18" customHeight="1">
-      <c r="D437" s="4"/>
-    </row>
-    <row r="448" spans="4:4" ht="18" customHeight="1">
-      <c r="D448" s="4"/>
-    </row>
-    <row r="459" spans="3:4" ht="18" customHeight="1">
-      <c r="D459" s="4"/>
-    </row>
-    <row r="461" spans="3:4" ht="18" customHeight="1">
-      <c r="C461" s="4"/>
-      <c r="D461" s="4"/>
-    </row>
-    <row r="467" spans="3:7" ht="18" customHeight="1">
-      <c r="G467" s="7"/>
-    </row>
-    <row r="475" spans="3:7" ht="18" customHeight="1">
-      <c r="C475" s="4"/>
-      <c r="D475" s="4"/>
-    </row>
-    <row r="487" spans="4:4" ht="18" customHeight="1">
-      <c r="D487" s="4"/>
-    </row>
-    <row r="512" spans="7:7" ht="18" customHeight="1">
-      <c r="G512" s="7"/>
-    </row>
-    <row r="517" spans="4:4" ht="18" customHeight="1">
-      <c r="D517" s="4"/>
-    </row>
-    <row r="520" spans="4:4" ht="18" customHeight="1">
-      <c r="D520" s="4"/>
-    </row>
-    <row r="522" spans="4:4" ht="18" customHeight="1">
-      <c r="D522" s="4"/>
-    </row>
-    <row r="526" spans="4:4" ht="18" customHeight="1">
-      <c r="D526" s="4"/>
-    </row>
-    <row r="532" spans="3:4" ht="18" customHeight="1">
-      <c r="D532" s="4"/>
-    </row>
-    <row r="536" spans="3:4" ht="18" customHeight="1">
-      <c r="C536" s="4"/>
-      <c r="D536" s="4"/>
-    </row>
-    <row r="548" spans="3:7" ht="18" customHeight="1">
-      <c r="C548" s="4"/>
-      <c r="D548" s="4"/>
-    </row>
-    <row r="550" spans="3:7" ht="18" customHeight="1">
-      <c r="C550" s="4"/>
-      <c r="D550" s="4"/>
-    </row>
-    <row r="557" spans="3:7" ht="18" customHeight="1">
-      <c r="G557" s="7"/>
-    </row>
-    <row r="574" spans="3:4" ht="18" customHeight="1">
-      <c r="C574" s="4"/>
-      <c r="D574" s="4"/>
-    </row>
-    <row r="575" spans="3:4" ht="18" customHeight="1">
-      <c r="C575" s="4"/>
-      <c r="D575" s="4"/>
-    </row>
-    <row r="579" spans="3:4" ht="18" customHeight="1">
-      <c r="D579" s="4"/>
-    </row>
-    <row r="581" spans="3:4" ht="18" customHeight="1">
-      <c r="C581" s="4"/>
-      <c r="D581" s="4"/>
-    </row>
-    <row r="588" spans="3:4" ht="18" customHeight="1">
-      <c r="C588" s="4"/>
-      <c r="D588" s="4"/>
-    </row>
-    <row r="602" spans="3:7" ht="18" customHeight="1">
-      <c r="G602" s="7"/>
-    </row>
-    <row r="606" spans="3:7" ht="18" customHeight="1">
-      <c r="C606" s="4"/>
-      <c r="D606" s="4"/>
-    </row>
-    <row r="617" spans="3:4" ht="18" customHeight="1">
-      <c r="C617" s="4"/>
-      <c r="D617" s="4"/>
-    </row>
-    <row r="622" spans="3:4" ht="18" customHeight="1">
-      <c r="D622" s="4"/>
-    </row>
-    <row r="623" spans="3:4" ht="18" customHeight="1">
-      <c r="D623" s="4"/>
-    </row>
-    <row r="626" spans="3:4" ht="18" customHeight="1">
-      <c r="C626" s="4"/>
-      <c r="D626" s="4"/>
-    </row>
-    <row r="639" spans="3:4" ht="18" customHeight="1">
-      <c r="D639" s="4"/>
-    </row>
-    <row r="647" spans="7:7" ht="18" customHeight="1">
-      <c r="G647" s="7"/>
-    </row>
-    <row r="657" spans="3:4" ht="18" customHeight="1">
-      <c r="D657" s="4"/>
-    </row>
-    <row r="659" spans="3:4" ht="18" customHeight="1">
-      <c r="C659" s="4"/>
-      <c r="D659" s="4"/>
-    </row>
-    <row r="660" spans="3:4" ht="18" customHeight="1">
-      <c r="C660" s="4"/>
-      <c r="D660" s="4"/>
-    </row>
-    <row r="663" spans="3:4" ht="18" customHeight="1">
-      <c r="C663" s="4"/>
-      <c r="D663" s="4"/>
-    </row>
-    <row r="664" spans="3:4" ht="18" customHeight="1">
-      <c r="C664" s="4"/>
-      <c r="D664" s="4"/>
-    </row>
-    <row r="692" spans="3:7" ht="18" customHeight="1">
-      <c r="G692" s="7"/>
-    </row>
-    <row r="698" spans="3:7" ht="18" customHeight="1">
-      <c r="C698" s="4"/>
-      <c r="D698" s="4"/>
-    </row>
-    <row r="699" spans="3:7" ht="18" customHeight="1">
-      <c r="D699" s="4"/>
-    </row>
-    <row r="710" spans="4:4" ht="18" customHeight="1">
-      <c r="D710" s="4"/>
-    </row>
-    <row r="724" spans="3:4" ht="18" customHeight="1">
-      <c r="D724" s="4"/>
+    <row r="260" spans="3:4" ht="18" customHeight="1">
+      <c r="D260" s="4"/>
+    </row>
+    <row r="269" spans="3:4" ht="18" customHeight="1">
+      <c r="C269" s="4"/>
+      <c r="D269" s="4"/>
+    </row>
+    <row r="272" spans="3:4" ht="18" customHeight="1">
+      <c r="D272" s="4"/>
+    </row>
+    <row r="291" spans="3:4" ht="18" customHeight="1">
+      <c r="C291" s="4"/>
+      <c r="D291" s="4"/>
+    </row>
+    <row r="305" spans="4:4" ht="18" customHeight="1">
+      <c r="D305" s="4"/>
+    </row>
+    <row r="329" spans="3:4" ht="18" customHeight="1">
+      <c r="C329" s="4"/>
+      <c r="D329" s="4"/>
+    </row>
+    <row r="333" spans="3:4" ht="18" customHeight="1">
+      <c r="D333" s="4"/>
+    </row>
+    <row r="336" spans="3:4" ht="18" customHeight="1">
+      <c r="C336" s="4"/>
+      <c r="D336" s="4"/>
+    </row>
+    <row r="337" spans="3:4" ht="18" customHeight="1">
+      <c r="C337" s="4"/>
+      <c r="D337" s="4"/>
+    </row>
+    <row r="347" spans="3:4" ht="18" customHeight="1">
+      <c r="C347" s="4"/>
+      <c r="D347" s="4"/>
+    </row>
+    <row r="376" spans="4:4" ht="18" customHeight="1">
+      <c r="D376" s="4"/>
+    </row>
+    <row r="385" spans="4:4" ht="18" customHeight="1">
+      <c r="D385" s="4"/>
+    </row>
+    <row r="387" spans="4:4" ht="18" customHeight="1">
+      <c r="D387" s="4"/>
+    </row>
+    <row r="390" spans="4:4" ht="18" customHeight="1">
+      <c r="D390" s="4"/>
+    </row>
+    <row r="395" spans="4:4" ht="18" customHeight="1">
+      <c r="D395" s="4"/>
+    </row>
+    <row r="396" spans="4:4" ht="18" customHeight="1">
+      <c r="D396" s="4"/>
+    </row>
+    <row r="405" spans="3:4" ht="18" customHeight="1">
+      <c r="C405" s="4"/>
+      <c r="D405" s="4"/>
+    </row>
+    <row r="414" spans="3:4" ht="18" customHeight="1">
+      <c r="D414" s="4"/>
+    </row>
+    <row r="425" spans="4:4" ht="18" customHeight="1">
+      <c r="D425" s="4"/>
+    </row>
+    <row r="436" spans="3:4" ht="18" customHeight="1">
+      <c r="D436" s="4"/>
+    </row>
+    <row r="438" spans="3:4" ht="18" customHeight="1">
+      <c r="C438" s="4"/>
+      <c r="D438" s="4"/>
+    </row>
+    <row r="452" spans="3:4" ht="18" customHeight="1">
+      <c r="C452" s="4"/>
+      <c r="D452" s="4"/>
+    </row>
+    <row r="464" spans="3:4" ht="18" customHeight="1">
+      <c r="D464" s="4"/>
+    </row>
+    <row r="494" spans="4:4" ht="18" customHeight="1">
+      <c r="D494" s="4"/>
+    </row>
+    <row r="497" spans="4:4" ht="18" customHeight="1">
+      <c r="D497" s="4"/>
+    </row>
+    <row r="499" spans="4:4" ht="18" customHeight="1">
+      <c r="D499" s="4"/>
+    </row>
+    <row r="503" spans="4:4" ht="18" customHeight="1">
+      <c r="D503" s="4"/>
+    </row>
+    <row r="509" spans="4:4" ht="18" customHeight="1">
+      <c r="D509" s="4"/>
+    </row>
+    <row r="513" spans="3:4" ht="18" customHeight="1">
+      <c r="C513" s="4"/>
+      <c r="D513" s="4"/>
+    </row>
+    <row r="525" spans="3:4" ht="18" customHeight="1">
+      <c r="C525" s="4"/>
+      <c r="D525" s="4"/>
+    </row>
+    <row r="527" spans="3:4" ht="18" customHeight="1">
+      <c r="C527" s="4"/>
+      <c r="D527" s="4"/>
+    </row>
+    <row r="551" spans="3:4" ht="18" customHeight="1">
+      <c r="C551" s="4"/>
+      <c r="D551" s="4"/>
+    </row>
+    <row r="552" spans="3:4" ht="18" customHeight="1">
+      <c r="C552" s="4"/>
+      <c r="D552" s="4"/>
+    </row>
+    <row r="556" spans="3:4" ht="18" customHeight="1">
+      <c r="D556" s="4"/>
+    </row>
+    <row r="558" spans="3:4" ht="18" customHeight="1">
+      <c r="C558" s="4"/>
+      <c r="D558" s="4"/>
+    </row>
+    <row r="565" spans="3:4" ht="18" customHeight="1">
+      <c r="C565" s="4"/>
+      <c r="D565" s="4"/>
+    </row>
+    <row r="583" spans="3:4" ht="18" customHeight="1">
+      <c r="C583" s="4"/>
+      <c r="D583" s="4"/>
+    </row>
+    <row r="594" spans="3:4" ht="18" customHeight="1">
+      <c r="C594" s="4"/>
+      <c r="D594" s="4"/>
+    </row>
+    <row r="599" spans="3:4" ht="18" customHeight="1">
+      <c r="D599" s="4"/>
+    </row>
+    <row r="600" spans="3:4" ht="18" customHeight="1">
+      <c r="D600" s="4"/>
+    </row>
+    <row r="603" spans="3:4" ht="18" customHeight="1">
+      <c r="C603" s="4"/>
+      <c r="D603" s="4"/>
+    </row>
+    <row r="616" spans="4:4" ht="18" customHeight="1">
+      <c r="D616" s="4"/>
+    </row>
+    <row r="634" spans="3:4" ht="18" customHeight="1">
+      <c r="D634" s="4"/>
+    </row>
+    <row r="636" spans="3:4" ht="18" customHeight="1">
+      <c r="C636" s="4"/>
+      <c r="D636" s="4"/>
+    </row>
+    <row r="637" spans="3:4" ht="18" customHeight="1">
+      <c r="C637" s="4"/>
+      <c r="D637" s="4"/>
+    </row>
+    <row r="640" spans="3:4" ht="18" customHeight="1">
+      <c r="C640" s="4"/>
+      <c r="D640" s="4"/>
+    </row>
+    <row r="641" spans="3:4" ht="18" customHeight="1">
+      <c r="C641" s="4"/>
+      <c r="D641" s="4"/>
+    </row>
+    <row r="675" spans="3:4" ht="18" customHeight="1">
+      <c r="C675" s="4"/>
+      <c r="D675" s="4"/>
+    </row>
+    <row r="676" spans="3:4" ht="18" customHeight="1">
+      <c r="D676" s="4"/>
+    </row>
+    <row r="687" spans="3:4" ht="18" customHeight="1">
+      <c r="D687" s="4"/>
+    </row>
+    <row r="701" spans="3:4" ht="18" customHeight="1">
+      <c r="D701" s="4"/>
+    </row>
+    <row r="703" spans="3:4" ht="18" customHeight="1">
+      <c r="C703" s="4"/>
+      <c r="D703" s="4"/>
     </row>
     <row r="726" spans="3:4" ht="18" customHeight="1">
       <c r="C726" s="4"/>
       <c r="D726" s="4"/>
     </row>
-    <row r="737" spans="3:7" ht="18" customHeight="1">
-      <c r="G737" s="7"/>
-    </row>
-    <row r="749" spans="3:7" ht="18" customHeight="1">
-      <c r="C749" s="4"/>
-      <c r="D749" s="4"/>
-    </row>
-    <row r="755" spans="3:4" ht="18" customHeight="1">
-      <c r="C755" s="4"/>
-      <c r="D755" s="4"/>
-    </row>
-    <row r="756" spans="3:4" ht="18" customHeight="1">
-      <c r="C756" s="4"/>
-      <c r="D756" s="4"/>
-    </row>
-    <row r="757" spans="3:4" ht="18" customHeight="1">
-      <c r="C757" s="4"/>
-      <c r="D757" s="4"/>
-    </row>
-    <row r="758" spans="3:4" ht="18" customHeight="1">
-      <c r="C758" s="4"/>
-      <c r="D758" s="4"/>
-    </row>
-    <row r="759" spans="3:4" ht="18" customHeight="1">
-      <c r="C759" s="4"/>
-      <c r="D759" s="4"/>
-    </row>
-    <row r="760" spans="3:4" ht="18" customHeight="1">
-      <c r="C760" s="4"/>
-      <c r="D760" s="4"/>
-    </row>
-    <row r="771" spans="4:7" ht="18" customHeight="1">
-      <c r="D771" s="4"/>
-    </row>
-    <row r="775" spans="4:7" ht="18" customHeight="1">
-      <c r="D775" s="4"/>
-    </row>
-    <row r="776" spans="4:7" ht="18" customHeight="1">
-      <c r="D776" s="4"/>
-    </row>
-    <row r="782" spans="4:7" ht="18" customHeight="1">
-      <c r="G782" s="7"/>
-    </row>
-    <row r="807" spans="3:4" ht="18" customHeight="1">
-      <c r="C807" s="4"/>
-      <c r="D807" s="4"/>
+    <row r="732" spans="3:4" ht="18" customHeight="1">
+      <c r="C732" s="4"/>
+      <c r="D732" s="4"/>
+    </row>
+    <row r="733" spans="3:4" ht="18" customHeight="1">
+      <c r="C733" s="4"/>
+      <c r="D733" s="4"/>
+    </row>
+    <row r="734" spans="3:4" ht="18" customHeight="1">
+      <c r="C734" s="4"/>
+      <c r="D734" s="4"/>
+    </row>
+    <row r="735" spans="3:4" ht="18" customHeight="1">
+      <c r="C735" s="4"/>
+      <c r="D735" s="4"/>
+    </row>
+    <row r="736" spans="3:4" ht="18" customHeight="1">
+      <c r="C736" s="4"/>
+      <c r="D736" s="4"/>
+    </row>
+    <row r="737" spans="3:4" ht="18" customHeight="1">
+      <c r="C737" s="4"/>
+      <c r="D737" s="4"/>
+    </row>
+    <row r="748" spans="3:4" ht="18" customHeight="1">
+      <c r="D748" s="4"/>
+    </row>
+    <row r="752" spans="3:4" ht="18" customHeight="1">
+      <c r="D752" s="4"/>
+    </row>
+    <row r="753" spans="4:4" ht="18" customHeight="1">
+      <c r="D753" s="4"/>
+    </row>
+    <row r="784" spans="3:4" ht="18" customHeight="1">
+      <c r="C784" s="4"/>
+      <c r="D784" s="4"/>
+    </row>
+    <row r="785" spans="3:4" ht="18" customHeight="1">
+      <c r="C785" s="4"/>
+      <c r="D785" s="4"/>
+    </row>
+    <row r="789" spans="3:4" ht="18" customHeight="1">
+      <c r="D789" s="4"/>
+    </row>
+    <row r="790" spans="3:4" ht="18" customHeight="1">
+      <c r="C790" s="4"/>
+      <c r="D790" s="4"/>
+    </row>
+    <row r="791" spans="3:4" ht="18" customHeight="1">
+      <c r="D791" s="4"/>
+    </row>
+    <row r="792" spans="3:4" ht="18" customHeight="1">
+      <c r="C792" s="4"/>
+      <c r="D792" s="4"/>
+    </row>
+    <row r="796" spans="3:4" ht="18" customHeight="1">
+      <c r="D796" s="4"/>
+    </row>
+    <row r="797" spans="3:4" ht="18" customHeight="1">
+      <c r="C797" s="4"/>
+      <c r="D797" s="4"/>
+    </row>
+    <row r="800" spans="3:4" ht="18" customHeight="1">
+      <c r="D800" s="4"/>
+    </row>
+    <row r="801" spans="3:4" ht="18" customHeight="1">
+      <c r="D801" s="4"/>
     </row>
     <row r="808" spans="3:4" ht="18" customHeight="1">
-      <c r="C808" s="4"/>
       <c r="D808" s="4"/>
     </row>
-    <row r="812" spans="3:4" ht="18" customHeight="1">
-      <c r="D812" s="4"/>
-    </row>
-    <row r="813" spans="3:4" ht="18" customHeight="1">
-      <c r="C813" s="4"/>
-      <c r="D813" s="4"/>
+    <row r="810" spans="3:4" ht="18" customHeight="1">
+      <c r="C810" s="4"/>
+      <c r="D810" s="4"/>
+    </row>
+    <row r="811" spans="3:4" ht="18" customHeight="1">
+      <c r="C811" s="4"/>
+      <c r="D811" s="4"/>
     </row>
     <row r="814" spans="3:4" ht="18" customHeight="1">
       <c r="D814" s="4"/>
     </row>
-    <row r="815" spans="3:4" ht="18" customHeight="1">
-      <c r="C815" s="4"/>
-      <c r="D815" s="4"/>
-    </row>
-    <row r="819" spans="3:7" ht="18" customHeight="1">
+    <row r="817" spans="4:4" ht="18" customHeight="1">
+      <c r="D817" s="4"/>
+    </row>
+    <row r="819" spans="4:4" ht="18" customHeight="1">
       <c r="D819" s="4"/>
-    </row>
-    <row r="820" spans="3:7" ht="18" customHeight="1">
-      <c r="C820" s="4"/>
-      <c r="D820" s="4"/>
-    </row>
-    <row r="823" spans="3:7" ht="18" customHeight="1">
-      <c r="D823" s="4"/>
-    </row>
-    <row r="824" spans="3:7" ht="18" customHeight="1">
-      <c r="D824" s="4"/>
-    </row>
-    <row r="827" spans="3:7" ht="18" customHeight="1">
-      <c r="G827" s="7"/>
-    </row>
-    <row r="831" spans="3:7" ht="18" customHeight="1">
-      <c r="D831" s="4"/>
-    </row>
-    <row r="833" spans="3:4" ht="18" customHeight="1">
-      <c r="C833" s="4"/>
-      <c r="D833" s="4"/>
     </row>
     <row r="834" spans="3:4" ht="18" customHeight="1">
       <c r="C834" s="4"/>
       <c r="D834" s="4"/>
     </row>
-    <row r="837" spans="3:4" ht="18" customHeight="1">
-      <c r="D837" s="4"/>
+    <row r="836" spans="3:4" ht="18" customHeight="1">
+      <c r="C836" s="4"/>
+      <c r="D836" s="4"/>
     </row>
     <row r="840" spans="3:4" ht="18" customHeight="1">
       <c r="D840" s="4"/>
     </row>
-    <row r="842" spans="3:4" ht="18" customHeight="1">
-      <c r="D842" s="4"/>
-    </row>
-    <row r="857" spans="3:4" ht="18" customHeight="1">
-      <c r="C857" s="4"/>
-      <c r="D857" s="4"/>
-    </row>
-    <row r="859" spans="3:4" ht="18" customHeight="1">
-      <c r="C859" s="4"/>
-      <c r="D859" s="4"/>
-    </row>
-    <row r="863" spans="3:4" ht="18" customHeight="1">
-      <c r="D863" s="4"/>
-    </row>
-    <row r="866" spans="3:7" ht="18" customHeight="1">
-      <c r="D866" s="4"/>
-    </row>
-    <row r="867" spans="3:7" ht="18" customHeight="1">
-      <c r="C867" s="4"/>
-      <c r="D867" s="4"/>
-    </row>
-    <row r="868" spans="3:7" ht="18" customHeight="1">
-      <c r="C868" s="4"/>
-      <c r="D868" s="4"/>
-    </row>
-    <row r="872" spans="3:7" ht="18" customHeight="1">
-      <c r="G872" s="7"/>
-    </row>
-    <row r="876" spans="3:7" ht="18" customHeight="1">
-      <c r="C876" s="4"/>
-      <c r="D876" s="4"/>
-    </row>
-    <row r="879" spans="3:7" ht="18" customHeight="1">
-      <c r="D879" s="4"/>
-    </row>
-    <row r="884" spans="3:4" ht="18" customHeight="1">
-      <c r="C884" s="4"/>
-      <c r="D884" s="4"/>
-    </row>
-    <row r="887" spans="3:4" ht="18" customHeight="1">
-      <c r="C887" s="4"/>
-      <c r="D887" s="4"/>
-    </row>
-    <row r="888" spans="3:4" ht="18" customHeight="1">
-      <c r="C888" s="4"/>
-      <c r="D888" s="4"/>
-    </row>
-    <row r="892" spans="3:4" ht="18" customHeight="1">
-      <c r="C892" s="4"/>
-      <c r="D892" s="4"/>
-    </row>
-    <row r="893" spans="3:4" ht="18" customHeight="1">
-      <c r="D893" s="4"/>
-    </row>
-    <row r="917" spans="3:7" ht="18" customHeight="1">
-      <c r="G917" s="7"/>
-    </row>
-    <row r="927" spans="3:7" ht="18" customHeight="1">
-      <c r="C927" s="4"/>
+    <row r="843" spans="3:4" ht="18" customHeight="1">
+      <c r="D843" s="4"/>
+    </row>
+    <row r="844" spans="3:4" ht="18" customHeight="1">
+      <c r="C844" s="4"/>
+      <c r="D844" s="4"/>
+    </row>
+    <row r="845" spans="3:4" ht="18" customHeight="1">
+      <c r="C845" s="4"/>
+      <c r="D845" s="4"/>
+    </row>
+    <row r="853" spans="3:4" ht="18" customHeight="1">
+      <c r="C853" s="4"/>
+      <c r="D853" s="4"/>
+    </row>
+    <row r="856" spans="3:4" ht="18" customHeight="1">
+      <c r="D856" s="4"/>
+    </row>
+    <row r="861" spans="3:4" ht="18" customHeight="1">
+      <c r="C861" s="4"/>
+      <c r="D861" s="4"/>
+    </row>
+    <row r="864" spans="3:4" ht="18" customHeight="1">
+      <c r="C864" s="4"/>
+      <c r="D864" s="4"/>
+    </row>
+    <row r="865" spans="3:4" ht="18" customHeight="1">
+      <c r="C865" s="4"/>
+      <c r="D865" s="4"/>
+    </row>
+    <row r="869" spans="3:4" ht="18" customHeight="1">
+      <c r="C869" s="4"/>
+      <c r="D869" s="4"/>
+    </row>
+    <row r="870" spans="3:4" ht="18" customHeight="1">
+      <c r="D870" s="4"/>
+    </row>
+    <row r="904" spans="3:4" ht="18" customHeight="1">
+      <c r="C904" s="4"/>
+      <c r="D904" s="4"/>
+    </row>
+    <row r="925" spans="3:4" ht="18" customHeight="1">
+      <c r="C925" s="4"/>
+      <c r="D925" s="4"/>
+    </row>
+    <row r="927" spans="3:4" ht="18" customHeight="1">
       <c r="D927" s="4"/>
     </row>
-    <row r="948" spans="3:4" ht="18" customHeight="1">
-      <c r="C948" s="4"/>
-      <c r="D948" s="4"/>
+    <row r="934" spans="3:4" ht="18" customHeight="1">
+      <c r="C934" s="4"/>
+      <c r="D934" s="4"/>
+    </row>
+    <row r="945" spans="3:4" ht="18" customHeight="1">
+      <c r="C945" s="4"/>
+      <c r="D945" s="4"/>
     </row>
     <row r="950" spans="3:4" ht="18" customHeight="1">
+      <c r="C950" s="4"/>
       <c r="D950" s="4"/>
     </row>
-    <row r="957" spans="3:4" ht="18" customHeight="1">
-      <c r="C957" s="4"/>
-      <c r="D957" s="4"/>
-    </row>
-    <row r="962" spans="3:7" ht="18" customHeight="1">
-      <c r="G962" s="7"/>
-    </row>
-    <row r="968" spans="3:7" ht="18" customHeight="1">
-      <c r="C968" s="4"/>
-      <c r="D968" s="4"/>
-    </row>
-    <row r="973" spans="3:7" ht="18" customHeight="1">
-      <c r="C973" s="4"/>
-      <c r="D973" s="4"/>
-    </row>
-    <row r="974" spans="3:7" ht="18" customHeight="1">
-      <c r="C974" s="4"/>
-      <c r="D974" s="4"/>
-    </row>
-    <row r="982" spans="3:4" ht="18" customHeight="1">
-      <c r="D982" s="4"/>
-    </row>
-    <row r="985" spans="3:4" ht="18" customHeight="1">
-      <c r="C985" s="4"/>
-      <c r="D985" s="4"/>
-    </row>
-    <row r="989" spans="3:4" ht="18" customHeight="1">
-      <c r="C989" s="4"/>
-      <c r="D989" s="4"/>
-    </row>
-    <row r="999" spans="3:7" ht="18" customHeight="1">
-      <c r="C999" s="4"/>
-      <c r="D999" s="4"/>
-    </row>
-    <row r="1000" spans="3:7" ht="18" customHeight="1">
-      <c r="C1000" s="4"/>
-      <c r="D1000" s="4"/>
-    </row>
-    <row r="1007" spans="3:7" ht="18" customHeight="1">
-      <c r="G1007" s="7"/>
+    <row r="951" spans="3:4" ht="18" customHeight="1">
+      <c r="C951" s="4"/>
+      <c r="D951" s="4"/>
+    </row>
+    <row r="959" spans="3:4" ht="18" customHeight="1">
+      <c r="D959" s="4"/>
+    </row>
+    <row r="962" spans="3:4" ht="18" customHeight="1">
+      <c r="C962" s="4"/>
+      <c r="D962" s="4"/>
+    </row>
+    <row r="966" spans="3:4" ht="18" customHeight="1">
+      <c r="C966" s="4"/>
+      <c r="D966" s="4"/>
+    </row>
+    <row r="976" spans="3:4" ht="18" customHeight="1">
+      <c r="C976" s="4"/>
+      <c r="D976" s="4"/>
+    </row>
+    <row r="977" spans="3:4" ht="18" customHeight="1">
+      <c r="C977" s="4"/>
+      <c r="D977" s="4"/>
+    </row>
+    <row r="994" spans="3:4" ht="18" customHeight="1">
+      <c r="C994" s="4"/>
+      <c r="D994" s="4"/>
+    </row>
+    <row r="995" spans="3:4" ht="18" customHeight="1">
+      <c r="C995" s="4"/>
+      <c r="D995" s="4"/>
+    </row>
+    <row r="1008" spans="3:4" ht="18" customHeight="1">
+      <c r="C1008" s="4"/>
+      <c r="D1008" s="4"/>
+    </row>
+    <row r="1009" spans="3:4" ht="18" customHeight="1">
+      <c r="C1009" s="4"/>
+      <c r="D1009" s="4"/>
+    </row>
+    <row r="1010" spans="3:4" ht="18" customHeight="1">
+      <c r="C1010" s="4"/>
+      <c r="D1010" s="4"/>
+    </row>
+    <row r="1011" spans="3:4" ht="18" customHeight="1">
+      <c r="C1011" s="4"/>
+      <c r="D1011" s="4"/>
+    </row>
+    <row r="1012" spans="3:4" ht="18" customHeight="1">
+      <c r="C1012" s="4"/>
+      <c r="D1012" s="4"/>
+    </row>
+    <row r="1013" spans="3:4" ht="18" customHeight="1">
+      <c r="C1013" s="4"/>
+      <c r="D1013" s="4"/>
+    </row>
+    <row r="1015" spans="3:4" ht="18" customHeight="1">
+      <c r="C1015" s="4"/>
+      <c r="D1015" s="4"/>
+    </row>
+    <row r="1016" spans="3:4" ht="18" customHeight="1">
+      <c r="C1016" s="4"/>
+      <c r="D1016" s="4"/>
     </row>
     <row r="1017" spans="3:4" ht="18" customHeight="1">
       <c r="C1017" s="4"/>
@@ -4038,356 +3945,347 @@
       <c r="C1018" s="4"/>
       <c r="D1018" s="4"/>
     </row>
-    <row r="1031" spans="3:4" ht="18" customHeight="1">
-      <c r="C1031" s="4"/>
-      <c r="D1031" s="4"/>
-    </row>
-    <row r="1032" spans="3:4" ht="18" customHeight="1">
-      <c r="C1032" s="4"/>
-      <c r="D1032" s="4"/>
+    <row r="1019" spans="3:4" ht="18" customHeight="1">
+      <c r="C1019" s="4"/>
+      <c r="D1019" s="4"/>
+    </row>
+    <row r="1020" spans="3:4" ht="18" customHeight="1">
+      <c r="C1020" s="4"/>
+      <c r="D1020" s="4"/>
+    </row>
+    <row r="1021" spans="3:4" ht="18" customHeight="1">
+      <c r="C1021" s="4"/>
+      <c r="D1021" s="4"/>
+    </row>
+    <row r="1022" spans="3:4" ht="18" customHeight="1">
+      <c r="C1022" s="4"/>
+      <c r="D1022" s="4"/>
+    </row>
+    <row r="1023" spans="3:4" ht="18" customHeight="1">
+      <c r="D1023" s="4"/>
+    </row>
+    <row r="1024" spans="3:4" ht="18" customHeight="1">
+      <c r="C1024" s="4"/>
+      <c r="D1024" s="4"/>
+    </row>
+    <row r="1025" spans="3:4" ht="18" customHeight="1">
+      <c r="C1025" s="4"/>
+      <c r="D1025" s="4"/>
+    </row>
+    <row r="1026" spans="3:4" ht="18" customHeight="1">
+      <c r="C1026" s="4"/>
+      <c r="D1026" s="4"/>
     </row>
     <row r="1033" spans="3:4" ht="18" customHeight="1">
       <c r="C1033" s="4"/>
       <c r="D1033" s="4"/>
     </row>
-    <row r="1034" spans="3:4" ht="18" customHeight="1">
-      <c r="C1034" s="4"/>
-      <c r="D1034" s="4"/>
-    </row>
     <row r="1035" spans="3:4" ht="18" customHeight="1">
-      <c r="C1035" s="4"/>
       <c r="D1035" s="4"/>
     </row>
-    <row r="1036" spans="3:4" ht="18" customHeight="1">
-      <c r="C1036" s="4"/>
-      <c r="D1036" s="4"/>
-    </row>
-    <row r="1038" spans="3:4" ht="18" customHeight="1">
-      <c r="C1038" s="4"/>
-      <c r="D1038" s="4"/>
-    </row>
-    <row r="1039" spans="3:4" ht="18" customHeight="1">
-      <c r="C1039" s="4"/>
-      <c r="D1039" s="4"/>
-    </row>
-    <row r="1040" spans="3:4" ht="18" customHeight="1">
-      <c r="C1040" s="4"/>
-      <c r="D1040" s="4"/>
-    </row>
-    <row r="1041" spans="3:7" ht="18" customHeight="1">
-      <c r="C1041" s="4"/>
-      <c r="D1041" s="4"/>
-    </row>
-    <row r="1042" spans="3:7" ht="18" customHeight="1">
-      <c r="C1042" s="4"/>
-      <c r="D1042" s="4"/>
-    </row>
-    <row r="1043" spans="3:7" ht="18" customHeight="1">
-      <c r="C1043" s="4"/>
-      <c r="D1043" s="4"/>
-    </row>
-    <row r="1044" spans="3:7" ht="18" customHeight="1">
-      <c r="C1044" s="4"/>
-      <c r="D1044" s="4"/>
-    </row>
-    <row r="1045" spans="3:7" ht="18" customHeight="1">
-      <c r="C1045" s="4"/>
-      <c r="D1045" s="4"/>
-    </row>
-    <row r="1046" spans="3:7" ht="18" customHeight="1">
-      <c r="D1046" s="4"/>
-    </row>
-    <row r="1047" spans="3:7" ht="18" customHeight="1">
-      <c r="C1047" s="4"/>
-      <c r="D1047" s="4"/>
-    </row>
-    <row r="1048" spans="3:7" ht="18" customHeight="1">
-      <c r="C1048" s="4"/>
-      <c r="D1048" s="4"/>
-    </row>
-    <row r="1049" spans="3:7" ht="18" customHeight="1">
-      <c r="C1049" s="4"/>
-      <c r="D1049" s="4"/>
-    </row>
-    <row r="1052" spans="3:7" ht="18" customHeight="1">
-      <c r="G1052" s="7"/>
-    </row>
-    <row r="1056" spans="3:7" ht="18" customHeight="1">
-      <c r="C1056" s="4"/>
-      <c r="D1056" s="4"/>
-    </row>
-    <row r="1058" spans="4:4" ht="18" customHeight="1">
-      <c r="D1058" s="4"/>
-    </row>
-    <row r="1083" spans="4:4" ht="18" customHeight="1">
-      <c r="D1083" s="4"/>
-    </row>
-    <row r="1084" spans="4:4" ht="18" customHeight="1">
-      <c r="D1084" s="4"/>
-    </row>
-    <row r="1085" spans="4:4" ht="18" customHeight="1">
-      <c r="D1085" s="4"/>
-    </row>
-    <row r="1088" spans="4:4" ht="18" customHeight="1">
+    <row r="1060" spans="3:4" ht="18" customHeight="1">
+      <c r="D1060" s="4"/>
+    </row>
+    <row r="1061" spans="3:4" ht="18" customHeight="1">
+      <c r="D1061" s="4"/>
+    </row>
+    <row r="1062" spans="3:4" ht="18" customHeight="1">
+      <c r="D1062" s="4"/>
+    </row>
+    <row r="1065" spans="3:4" ht="18" customHeight="1">
+      <c r="D1065" s="4"/>
+    </row>
+    <row r="1068" spans="3:4" ht="18" customHeight="1">
+      <c r="C1068" s="4"/>
+      <c r="D1068" s="4"/>
+    </row>
+    <row r="1078" spans="3:4" ht="18" customHeight="1">
+      <c r="C1078" s="4"/>
+      <c r="D1078" s="4"/>
+    </row>
+    <row r="1079" spans="3:4" ht="18" customHeight="1">
+      <c r="D1079" s="4"/>
+    </row>
+    <row r="1080" spans="3:4" ht="18" customHeight="1">
+      <c r="D1080" s="4"/>
+    </row>
+    <row r="1082" spans="3:4" ht="18" customHeight="1">
+      <c r="D1082" s="4"/>
+    </row>
+    <row r="1088" spans="3:4" ht="18" customHeight="1">
+      <c r="C1088" s="4"/>
       <c r="D1088" s="4"/>
     </row>
-    <row r="1091" spans="3:7" ht="18" customHeight="1">
-      <c r="C1091" s="4"/>
-      <c r="D1091" s="4"/>
-    </row>
-    <row r="1097" spans="3:7" ht="18" customHeight="1">
-      <c r="G1097" s="7"/>
-    </row>
-    <row r="1101" spans="3:7" ht="18" customHeight="1">
-      <c r="C1101" s="4"/>
-      <c r="D1101" s="4"/>
-    </row>
-    <row r="1102" spans="3:7" ht="18" customHeight="1">
+    <row r="1093" spans="3:4" ht="18" customHeight="1">
+      <c r="D1093" s="4"/>
+    </row>
+    <row r="1095" spans="3:4" ht="18" customHeight="1">
+      <c r="C1095" s="4"/>
+      <c r="D1095" s="4"/>
+    </row>
+    <row r="1099" spans="3:4" ht="18" customHeight="1">
+      <c r="C1099" s="4"/>
+      <c r="D1099" s="4"/>
+    </row>
+    <row r="1102" spans="3:4" ht="18" customHeight="1">
+      <c r="C1102" s="4"/>
       <c r="D1102" s="4"/>
     </row>
-    <row r="1103" spans="3:7" ht="18" customHeight="1">
-      <c r="D1103" s="4"/>
-    </row>
-    <row r="1105" spans="3:4" ht="18" customHeight="1">
-      <c r="D1105" s="4"/>
+    <row r="1106" spans="3:4" ht="18" customHeight="1">
+      <c r="C1106" s="4"/>
+      <c r="D1106" s="4"/>
+    </row>
+    <row r="1109" spans="3:4" ht="18" customHeight="1">
+      <c r="C1109" s="4"/>
+      <c r="D1109" s="4"/>
+    </row>
+    <row r="1110" spans="3:4" ht="18" customHeight="1">
+      <c r="D1110" s="4"/>
     </row>
     <row r="1111" spans="3:4" ht="18" customHeight="1">
-      <c r="C1111" s="4"/>
       <c r="D1111" s="4"/>
+    </row>
+    <row r="1114" spans="3:4" ht="18" customHeight="1">
+      <c r="C1114" s="4"/>
+      <c r="D1114" s="4"/>
+    </row>
+    <row r="1115" spans="3:4" ht="18" customHeight="1">
+      <c r="C1115" s="4"/>
+      <c r="D1115" s="4"/>
     </row>
     <row r="1116" spans="3:4" ht="18" customHeight="1">
       <c r="D1116" s="4"/>
     </row>
-    <row r="1118" spans="3:4" ht="18" customHeight="1">
-      <c r="C1118" s="4"/>
-      <c r="D1118" s="4"/>
-    </row>
-    <row r="1122" spans="3:4" ht="18" customHeight="1">
-      <c r="C1122" s="4"/>
-      <c r="D1122" s="4"/>
-    </row>
-    <row r="1125" spans="3:4" ht="18" customHeight="1">
-      <c r="C1125" s="4"/>
-      <c r="D1125" s="4"/>
-    </row>
-    <row r="1129" spans="3:4" ht="18" customHeight="1">
-      <c r="C1129" s="4"/>
-      <c r="D1129" s="4"/>
-    </row>
-    <row r="1132" spans="3:4" ht="18" customHeight="1">
-      <c r="C1132" s="4"/>
-      <c r="D1132" s="4"/>
-    </row>
-    <row r="1133" spans="3:4" ht="18" customHeight="1">
-      <c r="D1133" s="4"/>
-    </row>
-    <row r="1134" spans="3:4" ht="18" customHeight="1">
-      <c r="D1134" s="4"/>
-    </row>
-    <row r="1137" spans="3:7" ht="18" customHeight="1">
+    <row r="1126" spans="3:4" ht="18" customHeight="1">
+      <c r="D1126" s="4"/>
+    </row>
+    <row r="1136" spans="3:4" ht="18" customHeight="1">
+      <c r="C1136" s="4"/>
+      <c r="D1136" s="4"/>
+    </row>
+    <row r="1137" spans="3:4" ht="18" customHeight="1">
       <c r="C1137" s="4"/>
       <c r="D1137" s="4"/>
     </row>
-    <row r="1138" spans="3:7" ht="18" customHeight="1">
+    <row r="1138" spans="3:4" ht="18" customHeight="1">
       <c r="C1138" s="4"/>
       <c r="D1138" s="4"/>
     </row>
-    <row r="1139" spans="3:7" ht="18" customHeight="1">
+    <row r="1139" spans="3:4" ht="18" customHeight="1">
+      <c r="C1139" s="4"/>
       <c r="D1139" s="4"/>
     </row>
-    <row r="1142" spans="3:7" ht="18" customHeight="1">
-      <c r="G1142" s="7"/>
-    </row>
-    <row r="1149" spans="3:7" ht="18" customHeight="1">
-      <c r="D1149" s="4"/>
+    <row r="1140" spans="3:4" ht="18" customHeight="1">
+      <c r="D1140" s="4"/>
+    </row>
+    <row r="1141" spans="3:4" ht="18" customHeight="1">
+      <c r="C1141" s="4"/>
+      <c r="D1141" s="4"/>
+    </row>
+    <row r="1145" spans="3:4" ht="18" customHeight="1">
+      <c r="C1145" s="4"/>
+      <c r="D1145" s="4"/>
+    </row>
+    <row r="1146" spans="3:4" ht="18" customHeight="1">
+      <c r="C1146" s="4"/>
+      <c r="D1146" s="4"/>
+    </row>
+    <row r="1147" spans="3:4" ht="18" customHeight="1">
+      <c r="C1147" s="4"/>
+      <c r="D1147" s="4"/>
+    </row>
+    <row r="1150" spans="3:4" ht="18" customHeight="1">
+      <c r="D1150" s="4"/>
+    </row>
+    <row r="1151" spans="3:4" ht="18" customHeight="1">
+      <c r="D1151" s="4"/>
+    </row>
+    <row r="1153" spans="3:4" ht="18" customHeight="1">
+      <c r="D1153" s="4"/>
+    </row>
+    <row r="1156" spans="3:4" ht="18" customHeight="1">
+      <c r="C1156" s="4"/>
+      <c r="D1156" s="4"/>
     </row>
     <row r="1159" spans="3:4" ht="18" customHeight="1">
       <c r="C1159" s="4"/>
       <c r="D1159" s="4"/>
     </row>
-    <row r="1160" spans="3:4" ht="18" customHeight="1">
-      <c r="C1160" s="4"/>
-      <c r="D1160" s="4"/>
-    </row>
     <row r="1161" spans="3:4" ht="18" customHeight="1">
       <c r="C1161" s="4"/>
       <c r="D1161" s="4"/>
     </row>
-    <row r="1162" spans="3:4" ht="18" customHeight="1">
-      <c r="C1162" s="4"/>
-      <c r="D1162" s="4"/>
-    </row>
-    <row r="1163" spans="3:4" ht="18" customHeight="1">
-      <c r="D1163" s="4"/>
-    </row>
-    <row r="1164" spans="3:4" ht="18" customHeight="1">
-      <c r="C1164" s="4"/>
-      <c r="D1164" s="4"/>
-    </row>
-    <row r="1168" spans="3:4" ht="18" customHeight="1">
-      <c r="C1168" s="4"/>
-      <c r="D1168" s="4"/>
-    </row>
-    <row r="1169" spans="3:4" ht="18" customHeight="1">
-      <c r="C1169" s="4"/>
-      <c r="D1169" s="4"/>
-    </row>
-    <row r="1170" spans="3:4" ht="18" customHeight="1">
-      <c r="C1170" s="4"/>
-      <c r="D1170" s="4"/>
+    <row r="1172" spans="3:4" ht="18" customHeight="1">
+      <c r="D1172" s="4"/>
     </row>
     <row r="1173" spans="3:4" ht="18" customHeight="1">
+      <c r="C1173" s="4"/>
       <c r="D1173" s="4"/>
     </row>
-    <row r="1174" spans="3:4" ht="18" customHeight="1">
-      <c r="D1174" s="4"/>
-    </row>
-    <row r="1176" spans="3:4" ht="18" customHeight="1">
-      <c r="D1176" s="4"/>
-    </row>
-    <row r="1179" spans="3:4" ht="18" customHeight="1">
-      <c r="C1179" s="4"/>
-      <c r="D1179" s="4"/>
-    </row>
-    <row r="1182" spans="3:4" ht="18" customHeight="1">
-      <c r="C1182" s="4"/>
-      <c r="D1182" s="4"/>
+    <row r="1177" spans="3:4" ht="18" customHeight="1">
+      <c r="C1177" s="4"/>
+      <c r="D1177" s="4"/>
+    </row>
+    <row r="1178" spans="3:4" ht="18" customHeight="1">
+      <c r="D1178" s="4"/>
+    </row>
+    <row r="1180" spans="3:4" ht="18" customHeight="1">
+      <c r="D1180" s="4"/>
+    </row>
+    <row r="1183" spans="3:4" ht="18" customHeight="1">
+      <c r="D1183" s="4"/>
     </row>
     <row r="1184" spans="3:4" ht="18" customHeight="1">
-      <c r="C1184" s="4"/>
       <c r="D1184" s="4"/>
     </row>
-    <row r="1187" spans="3:7" ht="18" customHeight="1">
-      <c r="G1187" s="7"/>
-    </row>
-    <row r="1195" spans="3:7" ht="18" customHeight="1">
+    <row r="1187" spans="3:4" ht="18" customHeight="1">
+      <c r="D1187" s="4"/>
+    </row>
+    <row r="1190" spans="3:4" ht="18" customHeight="1">
+      <c r="C1190" s="4"/>
+      <c r="D1190" s="4"/>
+    </row>
+    <row r="1191" spans="3:4" ht="18" customHeight="1">
+      <c r="C1191" s="4"/>
+      <c r="D1191" s="4"/>
+    </row>
+    <row r="1192" spans="3:4" ht="18" customHeight="1">
+      <c r="C1192" s="4"/>
+      <c r="D1192" s="4"/>
+    </row>
+    <row r="1193" spans="3:4" ht="18" customHeight="1">
+      <c r="C1193" s="4"/>
+      <c r="D1193" s="4"/>
+    </row>
+    <row r="1194" spans="3:4" ht="18" customHeight="1">
+      <c r="C1194" s="4"/>
+      <c r="D1194" s="4"/>
+    </row>
+    <row r="1195" spans="3:4" ht="18" customHeight="1">
+      <c r="C1195" s="4"/>
       <c r="D1195" s="4"/>
     </row>
-    <row r="1196" spans="3:7" ht="18" customHeight="1">
+    <row r="1196" spans="3:4" ht="18" customHeight="1">
       <c r="C1196" s="4"/>
       <c r="D1196" s="4"/>
     </row>
-    <row r="1200" spans="3:7" ht="18" customHeight="1">
+    <row r="1197" spans="3:4" ht="18" customHeight="1">
+      <c r="C1197" s="4"/>
+      <c r="D1197" s="4"/>
+    </row>
+    <row r="1198" spans="3:4" ht="18" customHeight="1">
+      <c r="C1198" s="4"/>
+      <c r="D1198" s="4"/>
+    </row>
+    <row r="1199" spans="3:4" ht="18" customHeight="1">
+      <c r="D1199" s="4"/>
+    </row>
+    <row r="1200" spans="3:4" ht="18" customHeight="1">
       <c r="C1200" s="4"/>
       <c r="D1200" s="4"/>
     </row>
     <row r="1201" spans="3:4" ht="18" customHeight="1">
+      <c r="C1201" s="4"/>
       <c r="D1201" s="4"/>
     </row>
+    <row r="1202" spans="3:4" ht="18" customHeight="1">
+      <c r="C1202" s="4"/>
+      <c r="D1202" s="4"/>
+    </row>
     <row r="1203" spans="3:4" ht="18" customHeight="1">
+      <c r="C1203" s="4"/>
       <c r="D1203" s="4"/>
     </row>
-    <row r="1206" spans="3:4" ht="18" customHeight="1">
-      <c r="D1206" s="4"/>
-    </row>
-    <row r="1207" spans="3:4" ht="18" customHeight="1">
-      <c r="D1207" s="4"/>
-    </row>
-    <row r="1210" spans="3:4" ht="18" customHeight="1">
-      <c r="D1210" s="4"/>
+    <row r="1205" spans="3:4" ht="18" customHeight="1">
+      <c r="C1205" s="4"/>
+      <c r="D1205" s="4"/>
     </row>
     <row r="1213" spans="3:4" ht="18" customHeight="1">
       <c r="C1213" s="4"/>
       <c r="D1213" s="4"/>
     </row>
-    <row r="1214" spans="3:4" ht="18" customHeight="1">
-      <c r="C1214" s="4"/>
-      <c r="D1214" s="4"/>
-    </row>
-    <row r="1215" spans="3:4" ht="18" customHeight="1">
-      <c r="C1215" s="4"/>
-      <c r="D1215" s="4"/>
-    </row>
-    <row r="1216" spans="3:4" ht="18" customHeight="1">
-      <c r="C1216" s="4"/>
-      <c r="D1216" s="4"/>
-    </row>
-    <row r="1217" spans="3:7" ht="18" customHeight="1">
+    <row r="1217" spans="3:4" ht="18" customHeight="1">
       <c r="C1217" s="4"/>
       <c r="D1217" s="4"/>
     </row>
-    <row r="1218" spans="3:7" ht="18" customHeight="1">
+    <row r="1218" spans="3:4" ht="18" customHeight="1">
       <c r="C1218" s="4"/>
       <c r="D1218" s="4"/>
     </row>
-    <row r="1219" spans="3:7" ht="18" customHeight="1">
-      <c r="C1219" s="4"/>
-      <c r="D1219" s="4"/>
-    </row>
-    <row r="1220" spans="3:7" ht="18" customHeight="1">
-      <c r="C1220" s="4"/>
-      <c r="D1220" s="4"/>
-    </row>
-    <row r="1221" spans="3:7" ht="18" customHeight="1">
-      <c r="C1221" s="4"/>
+    <row r="1221" spans="3:4" ht="18" customHeight="1">
       <c r="D1221" s="4"/>
     </row>
-    <row r="1222" spans="3:7" ht="18" customHeight="1">
-      <c r="D1222" s="4"/>
-    </row>
-    <row r="1223" spans="3:7" ht="18" customHeight="1">
-      <c r="C1223" s="4"/>
-      <c r="D1223" s="4"/>
-    </row>
-    <row r="1224" spans="3:7" ht="18" customHeight="1">
-      <c r="C1224" s="4"/>
-      <c r="D1224" s="4"/>
-    </row>
-    <row r="1225" spans="3:7" ht="18" customHeight="1">
+    <row r="1225" spans="3:4" ht="18" customHeight="1">
       <c r="C1225" s="4"/>
       <c r="D1225" s="4"/>
     </row>
-    <row r="1226" spans="3:7" ht="18" customHeight="1">
-      <c r="C1226" s="4"/>
-      <c r="D1226" s="4"/>
-    </row>
-    <row r="1228" spans="3:7" ht="18" customHeight="1">
-      <c r="C1228" s="4"/>
-      <c r="D1228" s="4"/>
-    </row>
-    <row r="1232" spans="3:7" ht="18" customHeight="1">
-      <c r="G1232" s="7"/>
+    <row r="1229" spans="3:4" ht="18" customHeight="1">
+      <c r="C1229" s="4"/>
+      <c r="D1229" s="4"/>
+    </row>
+    <row r="1230" spans="3:4" ht="18" customHeight="1">
+      <c r="D1230" s="4"/>
+    </row>
+    <row r="1232" spans="3:4" ht="18" customHeight="1">
+      <c r="C1232" s="4"/>
+      <c r="D1232" s="4"/>
+    </row>
+    <row r="1233" spans="3:4" ht="18" customHeight="1">
+      <c r="C1233" s="4"/>
+      <c r="D1233" s="4"/>
+    </row>
+    <row r="1234" spans="3:4" ht="18" customHeight="1">
+      <c r="D1234" s="4"/>
+    </row>
+    <row r="1235" spans="3:4" ht="18" customHeight="1">
+      <c r="C1235" s="4"/>
+      <c r="D1235" s="4"/>
     </row>
     <row r="1236" spans="3:4" ht="18" customHeight="1">
       <c r="C1236" s="4"/>
       <c r="D1236" s="4"/>
     </row>
+    <row r="1237" spans="3:4" ht="18" customHeight="1">
+      <c r="C1237" s="4"/>
+      <c r="D1237" s="4"/>
+    </row>
+    <row r="1238" spans="3:4" ht="18" customHeight="1">
+      <c r="C1238" s="4"/>
+      <c r="D1238" s="4"/>
+    </row>
+    <row r="1239" spans="3:4" ht="18" customHeight="1">
+      <c r="C1239" s="4"/>
+      <c r="D1239" s="4"/>
+    </row>
     <row r="1240" spans="3:4" ht="18" customHeight="1">
       <c r="C1240" s="4"/>
       <c r="D1240" s="4"/>
     </row>
-    <row r="1241" spans="3:4" ht="18" customHeight="1">
-      <c r="C1241" s="4"/>
-      <c r="D1241" s="4"/>
+    <row r="1243" spans="3:4" ht="18" customHeight="1">
+      <c r="D1243" s="4"/>
     </row>
     <row r="1244" spans="3:4" ht="18" customHeight="1">
       <c r="D1244" s="4"/>
     </row>
-    <row r="1248" spans="3:4" ht="18" customHeight="1">
-      <c r="C1248" s="4"/>
-      <c r="D1248" s="4"/>
-    </row>
-    <row r="1252" spans="3:4" ht="18" customHeight="1">
-      <c r="C1252" s="4"/>
-      <c r="D1252" s="4"/>
-    </row>
-    <row r="1253" spans="3:4" ht="18" customHeight="1">
-      <c r="D1253" s="4"/>
-    </row>
-    <row r="1255" spans="3:4" ht="18" customHeight="1">
-      <c r="C1255" s="4"/>
-      <c r="D1255" s="4"/>
-    </row>
-    <row r="1256" spans="3:4" ht="18" customHeight="1">
-      <c r="C1256" s="4"/>
-      <c r="D1256" s="4"/>
-    </row>
-    <row r="1257" spans="3:4" ht="18" customHeight="1">
-      <c r="D1257" s="4"/>
-    </row>
-    <row r="1258" spans="3:4" ht="18" customHeight="1">
-      <c r="C1258" s="4"/>
-      <c r="D1258" s="4"/>
+    <row r="1245" spans="3:4" ht="18" customHeight="1">
+      <c r="C1245" s="4"/>
+      <c r="D1245" s="4"/>
+    </row>
+    <row r="1246" spans="3:4" ht="18" customHeight="1">
+      <c r="C1246" s="4"/>
+      <c r="D1246" s="4"/>
+    </row>
+    <row r="1247" spans="3:4" ht="18" customHeight="1">
+      <c r="C1247" s="4"/>
+      <c r="D1247" s="4"/>
+    </row>
+    <row r="1250" spans="3:4" ht="18" customHeight="1">
+      <c r="C1250" s="4"/>
+      <c r="D1250" s="4"/>
+    </row>
+    <row r="1251" spans="3:4" ht="18" customHeight="1">
+      <c r="C1251" s="4"/>
+      <c r="D1251" s="4"/>
     </row>
     <row r="1259" spans="3:4" ht="18" customHeight="1">
       <c r="C1259" s="4"/>
@@ -4397,46 +4295,25 @@
       <c r="C1260" s="4"/>
       <c r="D1260" s="4"/>
     </row>
-    <row r="1261" spans="3:4" ht="18" customHeight="1">
-      <c r="C1261" s="4"/>
-      <c r="D1261" s="4"/>
-    </row>
     <row r="1262" spans="3:4" ht="18" customHeight="1">
       <c r="C1262" s="4"/>
       <c r="D1262" s="4"/>
     </row>
-    <row r="1263" spans="3:4" ht="18" customHeight="1">
-      <c r="C1263" s="4"/>
-      <c r="D1263" s="4"/>
-    </row>
-    <row r="1266" spans="3:7" ht="18" customHeight="1">
-      <c r="D1266" s="4"/>
-    </row>
-    <row r="1267" spans="3:7" ht="18" customHeight="1">
-      <c r="D1267" s="4"/>
-    </row>
-    <row r="1268" spans="3:7" ht="18" customHeight="1">
-      <c r="C1268" s="4"/>
-      <c r="D1268" s="4"/>
-    </row>
-    <row r="1269" spans="3:7" ht="18" customHeight="1">
+    <row r="1269" spans="3:4" ht="18" customHeight="1">
       <c r="C1269" s="4"/>
       <c r="D1269" s="4"/>
     </row>
-    <row r="1270" spans="3:7" ht="18" customHeight="1">
-      <c r="C1270" s="4"/>
-      <c r="D1270" s="4"/>
-    </row>
-    <row r="1273" spans="3:7" ht="18" customHeight="1">
-      <c r="C1273" s="4"/>
-      <c r="D1273" s="4"/>
-    </row>
-    <row r="1274" spans="3:7" ht="18" customHeight="1">
-      <c r="C1274" s="4"/>
-      <c r="D1274" s="4"/>
-    </row>
-    <row r="1277" spans="3:7" ht="18" customHeight="1">
-      <c r="G1277" s="7"/>
+    <row r="1271" spans="3:4" ht="18" customHeight="1">
+      <c r="C1271" s="4"/>
+      <c r="D1271" s="4"/>
+    </row>
+    <row r="1276" spans="3:4" ht="18" customHeight="1">
+      <c r="C1276" s="4"/>
+      <c r="D1276" s="4"/>
+    </row>
+    <row r="1281" spans="3:4" ht="18" customHeight="1">
+      <c r="C1281" s="4"/>
+      <c r="D1281" s="4"/>
     </row>
     <row r="1282" spans="3:4" ht="18" customHeight="1">
       <c r="C1282" s="4"/>
@@ -4447,132 +4324,98 @@
       <c r="D1283" s="4"/>
     </row>
     <row r="1285" spans="3:4" ht="18" customHeight="1">
-      <c r="C1285" s="4"/>
       <c r="D1285" s="4"/>
+    </row>
+    <row r="1286" spans="3:4" ht="18" customHeight="1">
+      <c r="D1286" s="4"/>
+    </row>
+    <row r="1287" spans="3:4" ht="18" customHeight="1">
+      <c r="C1287" s="4"/>
+      <c r="D1287" s="4"/>
+    </row>
+    <row r="1288" spans="3:4" ht="18" customHeight="1">
+      <c r="D1288" s="4"/>
+    </row>
+    <row r="1289" spans="3:4" ht="18" customHeight="1">
+      <c r="D1289" s="4"/>
+    </row>
+    <row r="1290" spans="3:4" ht="18" customHeight="1">
+      <c r="D1290" s="4"/>
+    </row>
+    <row r="1291" spans="3:4" ht="18" customHeight="1">
+      <c r="D1291" s="4"/>
     </row>
     <row r="1292" spans="3:4" ht="18" customHeight="1">
       <c r="C1292" s="4"/>
       <c r="D1292" s="4"/>
     </row>
     <row r="1294" spans="3:4" ht="18" customHeight="1">
-      <c r="C1294" s="4"/>
       <c r="D1294" s="4"/>
     </row>
-    <row r="1299" spans="3:4" ht="18" customHeight="1">
-      <c r="C1299" s="4"/>
-      <c r="D1299" s="4"/>
-    </row>
-    <row r="1304" spans="3:4" ht="18" customHeight="1">
-      <c r="C1304" s="4"/>
-      <c r="D1304" s="4"/>
-    </row>
-    <row r="1305" spans="3:4" ht="18" customHeight="1">
-      <c r="C1305" s="4"/>
-      <c r="D1305" s="4"/>
-    </row>
-    <row r="1306" spans="3:4" ht="18" customHeight="1">
-      <c r="C1306" s="4"/>
-      <c r="D1306" s="4"/>
-    </row>
-    <row r="1308" spans="3:4" ht="18" customHeight="1">
-      <c r="D1308" s="4"/>
-    </row>
-    <row r="1309" spans="3:4" ht="18" customHeight="1">
+    <row r="1307" spans="4:4" ht="18" customHeight="1">
+      <c r="D1307" s="4"/>
+    </row>
+    <row r="1309" spans="4:4" ht="18" customHeight="1">
       <c r="D1309" s="4"/>
     </row>
-    <row r="1310" spans="3:4" ht="18" customHeight="1">
-      <c r="C1310" s="4"/>
-      <c r="D1310" s="4"/>
-    </row>
-    <row r="1311" spans="3:4" ht="18" customHeight="1">
-      <c r="D1311" s="4"/>
-    </row>
-    <row r="1312" spans="3:4" ht="18" customHeight="1">
-      <c r="D1312" s="4"/>
-    </row>
-    <row r="1313" spans="3:7" ht="18" customHeight="1">
-      <c r="D1313" s="4"/>
-    </row>
-    <row r="1314" spans="3:7" ht="18" customHeight="1">
-      <c r="D1314" s="4"/>
-    </row>
-    <row r="1315" spans="3:7" ht="18" customHeight="1">
-      <c r="C1315" s="4"/>
-      <c r="D1315" s="4"/>
-    </row>
-    <row r="1317" spans="3:7" ht="18" customHeight="1">
-      <c r="D1317" s="4"/>
-    </row>
-    <row r="1322" spans="3:7" ht="18" customHeight="1">
-      <c r="G1322" s="7"/>
-    </row>
-    <row r="1330" spans="4:4" ht="18" customHeight="1">
-      <c r="D1330" s="4"/>
-    </row>
-    <row r="1332" spans="4:4" ht="18" customHeight="1">
-      <c r="D1332" s="4"/>
-    </row>
-    <row r="1344" spans="4:4" ht="18" customHeight="1">
-      <c r="D1344" s="4"/>
-    </row>
-    <row r="1345" spans="3:4" ht="18" customHeight="1">
-      <c r="C1345" s="4"/>
-      <c r="D1345" s="4"/>
-    </row>
-    <row r="1346" spans="3:4" ht="18" customHeight="1">
-      <c r="C1346" s="4"/>
-      <c r="D1346" s="4"/>
-    </row>
-    <row r="1347" spans="3:4" ht="18" customHeight="1">
-      <c r="C1347" s="4"/>
-      <c r="D1347" s="4"/>
-    </row>
-    <row r="1348" spans="3:4" ht="18" customHeight="1">
-      <c r="C1348" s="4"/>
-      <c r="D1348" s="4"/>
-    </row>
-    <row r="1349" spans="3:4" ht="18" customHeight="1">
-      <c r="C1349" s="4"/>
-      <c r="D1349" s="4"/>
-    </row>
-    <row r="1350" spans="3:4" ht="18" customHeight="1">
-      <c r="C1350" s="4"/>
-      <c r="D1350" s="4"/>
-    </row>
-    <row r="1351" spans="3:4" ht="18" customHeight="1">
-      <c r="C1351" s="4"/>
-      <c r="D1351" s="4"/>
-    </row>
-    <row r="1352" spans="3:4" ht="18" customHeight="1">
-      <c r="C1352" s="4"/>
-      <c r="D1352" s="4"/>
-    </row>
-    <row r="1354" spans="3:4" ht="18" customHeight="1">
-      <c r="C1354" s="4"/>
-      <c r="D1354" s="4"/>
-    </row>
-    <row r="1367" spans="7:7" ht="18" customHeight="1">
-      <c r="G1367" s="7"/>
-    </row>
-    <row r="1383" spans="3:5" ht="18" customHeight="1">
-      <c r="C1383" s="4"/>
-      <c r="D1383" s="4"/>
-    </row>
-    <row r="1385" spans="3:5" ht="18" customHeight="1">
-      <c r="C1385" s="4"/>
-      <c r="D1385" s="4"/>
-    </row>
-    <row r="1386" spans="3:5" ht="18" customHeight="1">
-      <c r="C1386" s="4"/>
-      <c r="D1386" s="4"/>
-    </row>
-    <row r="1388" spans="3:5" ht="18" customHeight="1">
-      <c r="C1388" s="4"/>
-      <c r="D1388" s="4"/>
-    </row>
-    <row r="1390" spans="3:5" ht="18" customHeight="1">
-      <c r="D1390" s="4"/>
-      <c r="E1390" s="5"/>
+    <row r="1321" spans="3:4" ht="18" customHeight="1">
+      <c r="D1321" s="4"/>
+    </row>
+    <row r="1322" spans="3:4" ht="18" customHeight="1">
+      <c r="C1322" s="4"/>
+      <c r="D1322" s="4"/>
+    </row>
+    <row r="1323" spans="3:4" ht="18" customHeight="1">
+      <c r="C1323" s="4"/>
+      <c r="D1323" s="4"/>
+    </row>
+    <row r="1324" spans="3:4" ht="18" customHeight="1">
+      <c r="C1324" s="4"/>
+      <c r="D1324" s="4"/>
+    </row>
+    <row r="1325" spans="3:4" ht="18" customHeight="1">
+      <c r="C1325" s="4"/>
+      <c r="D1325" s="4"/>
+    </row>
+    <row r="1326" spans="3:4" ht="18" customHeight="1">
+      <c r="C1326" s="4"/>
+      <c r="D1326" s="4"/>
+    </row>
+    <row r="1327" spans="3:4" ht="18" customHeight="1">
+      <c r="C1327" s="4"/>
+      <c r="D1327" s="4"/>
+    </row>
+    <row r="1328" spans="3:4" ht="18" customHeight="1">
+      <c r="C1328" s="4"/>
+      <c r="D1328" s="4"/>
+    </row>
+    <row r="1329" spans="3:4" ht="18" customHeight="1">
+      <c r="C1329" s="4"/>
+      <c r="D1329" s="4"/>
+    </row>
+    <row r="1331" spans="3:4" ht="18" customHeight="1">
+      <c r="C1331" s="4"/>
+      <c r="D1331" s="4"/>
+    </row>
+    <row r="1360" spans="3:4" ht="18" customHeight="1">
+      <c r="C1360" s="4"/>
+      <c r="D1360" s="4"/>
+    </row>
+    <row r="1362" spans="3:5" ht="18" customHeight="1">
+      <c r="C1362" s="4"/>
+      <c r="D1362" s="4"/>
+    </row>
+    <row r="1363" spans="3:5" ht="18" customHeight="1">
+      <c r="C1363" s="4"/>
+      <c r="D1363" s="4"/>
+    </row>
+    <row r="1365" spans="3:5" ht="18" customHeight="1">
+      <c r="C1365" s="4"/>
+      <c r="D1365" s="4"/>
+    </row>
+    <row r="1367" spans="3:5" ht="18" customHeight="1">
+      <c r="D1367" s="4"/>
+      <c r="E1367" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>